<commit_message>
ran on all pdfs
</commit_message>
<xml_diff>
--- a/data/qc_data/qc_reports_output/PO166939-204865/pdf_data/data.xlsx
+++ b/data/qc_data/qc_reports_output/PO166939-204865/pdf_data/data.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
-  <si>
-    <t>pdf_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="87">
   <si>
     <t>product_name</t>
   </si>
@@ -145,7 +142,7 @@
     <t>packs_fruits_inspected_sample_size</t>
   </si>
   <si>
-    <t>PO166939-204865</t>
+    <t>boxes_inspected</t>
   </si>
   <si>
     <t>Apricots 20x320g Punnet</t>
@@ -349,49 +346,49 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:AQ11" totalsRowShown="0">
   <autoFilter ref="A1:AQ11"/>
   <tableColumns count="43">
-    <tableColumn id="1" name="pdf_id" dataDxfId="0"/>
-    <tableColumn id="2" name="product_name" dataDxfId="0"/>
-    <tableColumn id="3" name="RAG" dataDxfId="0"/>
-    <tableColumn id="4" name="expected_qty" dataDxfId="0"/>
-    <tableColumn id="5" name="received_qty" dataDxfId="0"/>
-    <tableColumn id="6" name="supplier_code" dataDxfId="0"/>
-    <tableColumn id="7" name="supplier" dataDxfId="0"/>
-    <tableColumn id="8" name="coo" dataDxfId="0"/>
-    <tableColumn id="9" name="received_date" dataDxfId="0"/>
-    <tableColumn id="10" name="inspection_date" dataDxfId="0"/>
-    <tableColumn id="11" name="print_date" dataDxfId="0"/>
-    <tableColumn id="12" name="iss_pallet_id" dataDxfId="1"/>
-    <tableColumn id="13" name="supplier_pallet_id" dataDxfId="1"/>
-    <tableColumn id="14" name="customer_pallet_id" dataDxfId="1"/>
-    <tableColumn id="15" name="variety" dataDxfId="0"/>
-    <tableColumn id="16" name="brand" dataDxfId="0"/>
-    <tableColumn id="17" name="organic" dataDxfId="0"/>
-    <tableColumn id="18" name="does_pallet_meet_spec" dataDxfId="0"/>
-    <tableColumn id="19" name="end_customer" dataDxfId="0"/>
-    <tableColumn id="20" name="harvest_date" dataDxfId="0"/>
-    <tableColumn id="21" name="dp" dataDxfId="1"/>
-    <tableColumn id="22" name="total_defects_percentage" dataDxfId="2"/>
-    <tableColumn id="23" name="size_calibre" dataDxfId="0"/>
-    <tableColumn id="24" name="lot_number" dataDxfId="1"/>
-    <tableColumn id="25" name="inspector" dataDxfId="0"/>
-    <tableColumn id="26" name="estimated_yield_percentage" dataDxfId="2"/>
-    <tableColumn id="27" name="defects_fruit_total" dataDxfId="1"/>
-    <tableColumn id="28" name="packs_with_defects" dataDxfId="1"/>
-    <tableColumn id="29" name="waste_tot" dataDxfId="2"/>
-    <tableColumn id="30" name="waste_fruit_total" dataDxfId="1"/>
-    <tableColumn id="31" name="packs_with_waste" dataDxfId="1"/>
-    <tableColumn id="32" name="minor_defects_tot" dataDxfId="2"/>
-    <tableColumn id="33" name="minor_fruit_total" dataDxfId="1"/>
-    <tableColumn id="34" name="major_defects_tot" dataDxfId="2"/>
-    <tableColumn id="35" name="major_fruit_total" dataDxfId="1"/>
-    <tableColumn id="36" name="packs_with_major" dataDxfId="1"/>
-    <tableColumn id="37" name="box_pack_weights" dataDxfId="0"/>
-    <tableColumn id="38" name="under_weight_percentage" dataDxfId="2"/>
-    <tableColumn id="39" name="weight_readings" dataDxfId="0"/>
-    <tableColumn id="40" name="fruit_weights" dataDxfId="0"/>
-    <tableColumn id="41" name="under_size_percentage" dataDxfId="2"/>
-    <tableColumn id="42" name="qa_comments" dataDxfId="0"/>
-    <tableColumn id="43" name="packs_fruits_inspected_sample_size" dataDxfId="1"/>
+    <tableColumn id="1" name="product_name" dataDxfId="0"/>
+    <tableColumn id="2" name="RAG" dataDxfId="0"/>
+    <tableColumn id="3" name="expected_qty" dataDxfId="0"/>
+    <tableColumn id="4" name="received_qty" dataDxfId="0"/>
+    <tableColumn id="5" name="supplier_code" dataDxfId="0"/>
+    <tableColumn id="6" name="supplier" dataDxfId="0"/>
+    <tableColumn id="7" name="coo" dataDxfId="0"/>
+    <tableColumn id="8" name="received_date" dataDxfId="0"/>
+    <tableColumn id="9" name="inspection_date" dataDxfId="0"/>
+    <tableColumn id="10" name="print_date" dataDxfId="0"/>
+    <tableColumn id="11" name="iss_pallet_id" dataDxfId="1"/>
+    <tableColumn id="12" name="supplier_pallet_id" dataDxfId="1"/>
+    <tableColumn id="13" name="customer_pallet_id" dataDxfId="1"/>
+    <tableColumn id="14" name="variety" dataDxfId="0"/>
+    <tableColumn id="15" name="brand" dataDxfId="0"/>
+    <tableColumn id="16" name="organic" dataDxfId="0"/>
+    <tableColumn id="17" name="does_pallet_meet_spec" dataDxfId="0"/>
+    <tableColumn id="18" name="end_customer" dataDxfId="0"/>
+    <tableColumn id="19" name="harvest_date" dataDxfId="0"/>
+    <tableColumn id="20" name="dp" dataDxfId="1"/>
+    <tableColumn id="21" name="total_defects_percentage" dataDxfId="2"/>
+    <tableColumn id="22" name="size_calibre" dataDxfId="0"/>
+    <tableColumn id="23" name="lot_number" dataDxfId="1"/>
+    <tableColumn id="24" name="inspector" dataDxfId="0"/>
+    <tableColumn id="25" name="estimated_yield_percentage" dataDxfId="2"/>
+    <tableColumn id="26" name="defects_fruit_total" dataDxfId="1"/>
+    <tableColumn id="27" name="packs_with_defects" dataDxfId="1"/>
+    <tableColumn id="28" name="waste_tot" dataDxfId="2"/>
+    <tableColumn id="29" name="waste_fruit_total" dataDxfId="1"/>
+    <tableColumn id="30" name="packs_with_waste" dataDxfId="1"/>
+    <tableColumn id="31" name="minor_defects_tot" dataDxfId="2"/>
+    <tableColumn id="32" name="minor_fruit_total" dataDxfId="1"/>
+    <tableColumn id="33" name="major_defects_tot" dataDxfId="2"/>
+    <tableColumn id="34" name="major_fruit_total" dataDxfId="1"/>
+    <tableColumn id="35" name="packs_with_major" dataDxfId="1"/>
+    <tableColumn id="36" name="box_pack_weights" dataDxfId="0"/>
+    <tableColumn id="37" name="under_weight_percentage" dataDxfId="2"/>
+    <tableColumn id="38" name="weight_readings" dataDxfId="0"/>
+    <tableColumn id="39" name="fruit_weights" dataDxfId="0"/>
+    <tableColumn id="40" name="under_size_percentage" dataDxfId="2"/>
+    <tableColumn id="41" name="qa_comments" dataDxfId="0"/>
+    <tableColumn id="42" name="packs_fruits_inspected_sample_size" dataDxfId="1"/>
+    <tableColumn id="43" name="boxes_inspected" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -830,7 +827,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>46</v>
@@ -850,17 +847,17 @@
       <c r="J2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>52</v>
+      <c r="K2" s="2">
+        <v>7761770</v>
       </c>
       <c r="L2" s="2">
-        <v>7761770</v>
+        <v>5808239</v>
       </c>
       <c r="M2" s="2">
         <v>5808239</v>
       </c>
-      <c r="N2" s="2">
-        <v>5808239</v>
+      <c r="N2" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>53</v>
@@ -877,77 +874,77 @@
       <c r="S2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="2">
+        <v>7</v>
+      </c>
+      <c r="U2" s="3">
+        <v>5</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="2">
-        <v>7</v>
-      </c>
-      <c r="V2" s="3">
-        <v>5</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="2">
+        <v>508164</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="2">
-        <v>508164</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AK2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="AL2" s="3">
-        <v>0</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AN2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AO2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>64</v>
+      <c r="AP2" s="2">
+        <v>60</v>
       </c>
       <c r="AQ2" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -955,13 +952,13 @@
         <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>46</v>
@@ -981,17 +978,17 @@
       <c r="J3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>52</v>
+      <c r="K3" s="2">
+        <v>7761771</v>
       </c>
       <c r="L3" s="2">
-        <v>7761771</v>
+        <v>5808238</v>
       </c>
       <c r="M3" s="2">
         <v>5808238</v>
       </c>
-      <c r="N3" s="2">
-        <v>5808238</v>
+      <c r="N3" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>53</v>
@@ -1008,77 +1005,77 @@
       <c r="S3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="2">
+        <v>7</v>
+      </c>
+      <c r="U3" s="3">
+        <v>10.83</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="2">
-        <v>7</v>
-      </c>
-      <c r="V3" s="3">
-        <v>10.83</v>
-      </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="2">
+        <v>508165</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="2">
-        <v>508165</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z3" s="3">
+      <c r="Y3" s="3">
         <v>94</v>
       </c>
+      <c r="Z3" s="2">
+        <v>0</v>
+      </c>
       <c r="AA3" s="2">
         <v>0</v>
       </c>
-      <c r="AB3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="3">
+      <c r="AB3" s="3">
         <v>2.5</v>
       </c>
+      <c r="AC3" s="2">
+        <v>3</v>
+      </c>
       <c r="AD3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
         <v>5</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AF3" s="2">
         <v>6</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AG3" s="3">
         <v>3.33</v>
       </c>
+      <c r="AH3" s="2">
+        <v>4</v>
+      </c>
       <c r="AI3" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AL3" s="3">
-        <v>0</v>
-      </c>
       <c r="AM3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>68</v>
+      <c r="AP3" s="2">
+        <v>120</v>
       </c>
       <c r="AQ3" s="2">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -1092,7 +1089,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>46</v>
@@ -1112,16 +1109,16 @@
       <c r="J4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>52</v>
+      <c r="K4" s="2">
+        <v>7763099</v>
       </c>
       <c r="L4" s="2">
         <v>7763099</v>
       </c>
-      <c r="M4" s="2">
-        <v>7763099</v>
-      </c>
-      <c r="N4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1137,77 +1134,77 @@
       <c r="S4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="2">
+        <v>7</v>
+      </c>
+      <c r="U4" s="3">
+        <v>5</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="2">
-        <v>7</v>
-      </c>
-      <c r="V4" s="3">
-        <v>5</v>
-      </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="2">
+        <v>508164</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="2">
-        <v>508164</v>
-      </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP4" s="2">
         <v>60</v>
       </c>
-      <c r="Z4" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH4" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ4" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -1221,7 +1218,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>46</v>
@@ -1241,16 +1238,16 @@
       <c r="J5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>52</v>
+      <c r="K5" s="2">
+        <v>7763100</v>
       </c>
       <c r="L5" s="2">
         <v>7763100</v>
       </c>
-      <c r="M5" s="2">
-        <v>7763100</v>
-      </c>
-      <c r="N5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>53</v>
       </c>
@@ -1266,77 +1263,77 @@
       <c r="S5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="2">
+        <v>7</v>
+      </c>
+      <c r="U5" s="3">
+        <v>5</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="2">
-        <v>7</v>
-      </c>
-      <c r="V5" s="3">
-        <v>5</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="2">
+        <v>508164</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X5" s="2">
-        <v>508164</v>
-      </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP5" s="2">
         <v>60</v>
       </c>
-      <c r="Z5" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ5" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -1350,7 +1347,7 @@
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>46</v>
@@ -1370,16 +1367,16 @@
       <c r="J6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>52</v>
+      <c r="K6" s="2">
+        <v>7763101</v>
       </c>
       <c r="L6" s="2">
         <v>7763101</v>
       </c>
-      <c r="M6" s="2">
-        <v>7763101</v>
-      </c>
-      <c r="N6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1395,77 +1392,77 @@
       <c r="S6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="2">
+        <v>7</v>
+      </c>
+      <c r="U6" s="3">
+        <v>5</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U6" s="2">
-        <v>7</v>
-      </c>
-      <c r="V6" s="3">
-        <v>5</v>
-      </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="2">
+        <v>508164</v>
+      </c>
+      <c r="X6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X6" s="2">
-        <v>508164</v>
-      </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP6" s="2">
         <v>60</v>
       </c>
-      <c r="Z6" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH6" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AQ6" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -1473,13 +1470,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>46</v>
@@ -1499,16 +1496,16 @@
       <c r="J7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>52</v>
+      <c r="K7" s="2">
+        <v>7763102</v>
       </c>
       <c r="L7" s="2">
         <v>7763102</v>
       </c>
-      <c r="M7" s="2">
-        <v>7763102</v>
-      </c>
-      <c r="N7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O7" s="1" t="s">
         <v>53</v>
       </c>
@@ -1524,77 +1521,77 @@
       <c r="S7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U7" s="2">
+      <c r="T7" s="2">
         <v>7</v>
       </c>
-      <c r="V7" s="3">
+      <c r="U7" s="3">
         <v>10.83</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="V7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="2">
+        <v>508164</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>94</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>6</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="X7" s="2">
-        <v>508164</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>94</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3">
-        <v>5</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>6</v>
-      </c>
-      <c r="AH7" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AI7" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AK7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AL7" s="3">
-        <v>0</v>
-      </c>
       <c r="AM7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="AN7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>120</v>
       </c>
       <c r="AQ7" s="2">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -1608,7 +1605,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>46</v>
@@ -1628,16 +1625,16 @@
       <c r="J8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>52</v>
+      <c r="K8" s="2">
+        <v>7763103</v>
       </c>
       <c r="L8" s="2">
         <v>7763103</v>
       </c>
-      <c r="M8" s="2">
-        <v>7763103</v>
-      </c>
-      <c r="N8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O8" s="1" t="s">
         <v>53</v>
       </c>
@@ -1653,77 +1650,77 @@
       <c r="S8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U8" s="2">
+      <c r="T8" s="2">
         <v>7</v>
       </c>
-      <c r="V8" s="3">
+      <c r="U8" s="3">
         <v>5</v>
       </c>
-      <c r="W8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="X8" s="2">
+      <c r="V8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W8" s="2">
         <v>508164</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="X8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP8" s="2">
         <v>60</v>
       </c>
-      <c r="Z8" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH8" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="AQ8" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -1731,13 +1728,13 @@
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>46</v>
@@ -1757,16 +1754,16 @@
       <c r="J9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>52</v>
+      <c r="K9" s="2">
+        <v>7763104</v>
       </c>
       <c r="L9" s="2">
         <v>7763104</v>
       </c>
-      <c r="M9" s="2">
-        <v>7763104</v>
-      </c>
-      <c r="N9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O9" s="1" t="s">
         <v>53</v>
       </c>
@@ -1782,77 +1779,77 @@
       <c r="S9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U9" s="2">
+      <c r="T9" s="2">
         <v>7</v>
       </c>
-      <c r="V9" s="3">
+      <c r="U9" s="3">
         <v>10.83</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="X9" s="2">
+      <c r="V9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W9" s="2">
         <v>508164</v>
       </c>
-      <c r="Y9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z9" s="3">
+      <c r="X9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y9" s="3">
         <v>94</v>
       </c>
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
       <c r="AA9" s="2">
         <v>0</v>
       </c>
-      <c r="AB9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="3">
+      <c r="AB9" s="3">
         <v>2.5</v>
       </c>
+      <c r="AC9" s="2">
+        <v>3</v>
+      </c>
       <c r="AD9" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
         <v>5</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AF9" s="2">
         <v>6</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AG9" s="3">
         <v>3.33</v>
       </c>
+      <c r="AH9" s="2">
+        <v>4</v>
+      </c>
       <c r="AI9" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AL9" s="3">
-        <v>0</v>
-      </c>
       <c r="AM9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>120</v>
       </c>
       <c r="AQ9" s="2">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -1866,7 +1863,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>46</v>
@@ -1886,16 +1883,16 @@
       <c r="J10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>52</v>
+      <c r="K10" s="2">
+        <v>7763105</v>
       </c>
       <c r="L10" s="2">
         <v>7763105</v>
       </c>
-      <c r="M10" s="2">
-        <v>7763105</v>
-      </c>
-      <c r="N10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1911,77 +1908,77 @@
       <c r="S10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="2">
+        <v>7</v>
+      </c>
+      <c r="U10" s="3">
+        <v>5</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="2">
-        <v>7</v>
-      </c>
-      <c r="V10" s="3">
-        <v>5</v>
-      </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" s="2">
+        <v>508165</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X10" s="2">
-        <v>508165</v>
-      </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Y10" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP10" s="2">
         <v>60</v>
       </c>
-      <c r="Z10" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG10" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH10" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ10" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -1995,7 +1992,7 @@
         <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>46</v>
@@ -2015,16 +2012,16 @@
       <c r="J11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>52</v>
+      <c r="K11" s="2">
+        <v>7763106</v>
       </c>
       <c r="L11" s="2">
         <v>7763106</v>
       </c>
-      <c r="M11" s="2">
-        <v>7763106</v>
-      </c>
-      <c r="N11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="O11" s="1" t="s">
         <v>53</v>
       </c>
@@ -2040,77 +2037,77 @@
       <c r="S11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="2">
+        <v>7</v>
+      </c>
+      <c r="U11" s="3">
+        <v>5</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U11" s="2">
-        <v>7</v>
-      </c>
-      <c r="V11" s="3">
-        <v>5</v>
-      </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="2">
+        <v>508165</v>
+      </c>
+      <c r="X11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="2">
-        <v>508165</v>
-      </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Y11" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP11" s="2">
         <v>60</v>
       </c>
-      <c r="Z11" s="3">
-        <v>100</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="AG11" s="2">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="3">
-        <v>1.67</v>
-      </c>
-      <c r="AI11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AQ11" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>